<commit_message>
updated deprecated file names
</commit_message>
<xml_diff>
--- a/Dataset EV1.xlsx
+++ b/Dataset EV1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aurelien/Dropbox/COSMOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aurelien/Dropbox/COSMOS_MSB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7819255-2479-454F-AFC1-FB0B25B45E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB1AC50-9431-AF48-B5CB-502B70B16511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="17600" windowHeight="25420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,17 @@
     <sheet name="patient_sample_table" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1253,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="L3" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="O32" sqref="L25:O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>